<commit_message>
add examples and valueset
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-us-core-observation-sdoh-assessment.xlsx
+++ b/docs/StructureDefinition-us-core-observation-sdoh-assessment.xlsx
@@ -681,6 +681,9 @@
     <t>Knowing what kind of observation is being made is essential to understanding the observation.</t>
   </si>
   <si>
+    <t>extensible</t>
+  </si>
+  <si>
     <t>http://hl7.org/fhir/us/core/ValueSet/us-core-common-sdoh-assessments</t>
   </si>
   <si>
@@ -934,9 +937,6 @@
   </si>
   <si>
     <t>For many results it is necessary to handle exceptional values in measurements.</t>
-  </si>
-  <si>
-    <t>extensible</t>
   </si>
   <si>
     <t>Codes specifying why the result (`Observation.value[x]`) is missing.</t>
@@ -3885,11 +3885,11 @@
         <v>79</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>113</v>
+        <v>210</v>
       </c>
       <c r="X18" s="2"/>
       <c r="Y18" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="Z18" t="s" s="2">
         <v>79</v>
@@ -3922,27 +3922,27 @@
         <v>101</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AO18" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3965,19 +3965,19 @@
         <v>90</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>79</v>
@@ -4026,7 +4026,7 @@
         <v>79</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>77</v>
@@ -4041,19 +4041,19 @@
         <v>101</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>79</v>
@@ -4061,7 +4061,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -4084,16 +4084,16 @@
         <v>90</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -4143,7 +4143,7 @@
         <v>79</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>77</v>
@@ -4164,13 +4164,13 @@
         <v>79</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>79</v>
@@ -4178,11 +4178,11 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
@@ -4201,19 +4201,19 @@
         <v>90</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>79</v>
@@ -4262,7 +4262,7 @@
         <v>79</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>77</v>
@@ -4277,19 +4277,19 @@
         <v>101</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>79</v>
@@ -4297,11 +4297,11 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
@@ -4320,19 +4320,19 @@
         <v>90</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>79</v>
@@ -4381,7 +4381,7 @@
         <v>79</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>77</v>
@@ -4390,25 +4390,25 @@
         <v>89</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>79</v>
@@ -4416,7 +4416,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4439,16 +4439,16 @@
         <v>90</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
@@ -4498,7 +4498,7 @@
         <v>79</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>77</v>
@@ -4519,13 +4519,13 @@
         <v>79</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>79</v>
@@ -4533,7 +4533,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4556,19 +4556,19 @@
         <v>90</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>79</v>
@@ -4617,7 +4617,7 @@
         <v>79</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>77</v>
@@ -4632,19 +4632,19 @@
         <v>101</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AO24" t="s" s="2">
         <v>79</v>
@@ -4652,7 +4652,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4675,19 +4675,19 @@
         <v>90</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>79</v>
@@ -4736,7 +4736,7 @@
         <v>79</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>77</v>
@@ -4745,7 +4745,7 @@
         <v>89</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>101</v>
@@ -4754,24 +4754,24 @@
         <v>79</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4797,16 +4797,16 @@
         <v>187</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>79</v>
@@ -4831,7 +4831,7 @@
         <v>79</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>291</v>
+        <v>210</v>
       </c>
       <c r="X26" t="s" s="2">
         <v>292</v>
@@ -4855,7 +4855,7 @@
         <v>79</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>77</v>
@@ -4950,7 +4950,7 @@
         <v>79</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>291</v>
+        <v>210</v>
       </c>
       <c r="X27" t="s" s="2">
         <v>302</v>
@@ -7577,13 +7577,13 @@
         <v>442</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>79</v>
@@ -7614,19 +7614,19 @@
         <v>90</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="K50" t="s" s="2">
         <v>444</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="M50" t="s" s="2">
         <v>445</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>79</v>
@@ -7696,16 +7696,16 @@
         <v>446</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="51" hidden="true">
@@ -7745,7 +7745,7 @@
         <v>450</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>79</v>
@@ -7770,7 +7770,7 @@
         <v>79</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>291</v>
+        <v>210</v>
       </c>
       <c r="X51" t="s" s="2">
         <v>292</v>
@@ -7889,7 +7889,7 @@
         <v>79</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>291</v>
+        <v>210</v>
       </c>
       <c r="X52" t="s" s="2">
         <v>302</v>

</xml_diff>

<commit_message>
mock up for CGP call
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-us-core-observation-sdoh-assessment.xlsx
+++ b/docs/StructureDefinition-us-core-observation-sdoh-assessment.xlsx
@@ -681,9 +681,6 @@
     <t>Knowing what kind of observation is being made is essential to understanding the observation.</t>
   </si>
   <si>
-    <t>extensible</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/core/ValueSet/us-core-common-sdoh-assessments</t>
   </si>
   <si>
@@ -937,6 +934,9 @@
   </si>
   <si>
     <t>For many results it is necessary to handle exceptional values in measurements.</t>
+  </si>
+  <si>
+    <t>extensible</t>
   </si>
   <si>
     <t>Codes specifying why the result (`Observation.value[x]`) is missing.</t>
@@ -3885,11 +3885,11 @@
         <v>79</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>210</v>
+        <v>113</v>
       </c>
       <c r="X18" s="2"/>
       <c r="Y18" t="s" s="2">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Z18" t="s" s="2">
         <v>79</v>
@@ -3922,27 +3922,27 @@
         <v>101</v>
       </c>
       <c r="AJ18" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="AK18" t="s" s="2">
         <v>212</v>
       </c>
-      <c r="AK18" t="s" s="2">
+      <c r="AL18" t="s" s="2">
         <v>213</v>
       </c>
-      <c r="AL18" t="s" s="2">
+      <c r="AM18" t="s" s="2">
         <v>214</v>
       </c>
-      <c r="AM18" t="s" s="2">
+      <c r="AN18" t="s" s="2">
         <v>215</v>
       </c>
-      <c r="AN18" t="s" s="2">
+      <c r="AO18" t="s" s="2">
         <v>216</v>
-      </c>
-      <c r="AO18" t="s" s="2">
-        <v>217</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3965,19 +3965,19 @@
         <v>90</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="K19" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="K19" t="s" s="2">
+      <c r="L19" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="M19" t="s" s="2">
         <v>221</v>
       </c>
-      <c r="M19" t="s" s="2">
+      <c r="N19" t="s" s="2">
         <v>222</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>223</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>79</v>
@@ -4026,7 +4026,7 @@
         <v>79</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>77</v>
@@ -4041,19 +4041,19 @@
         <v>101</v>
       </c>
       <c r="AJ19" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="AK19" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AL19" t="s" s="2">
         <v>224</v>
       </c>
-      <c r="AK19" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AL19" t="s" s="2">
+      <c r="AM19" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="AM19" t="s" s="2">
+      <c r="AN19" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="AN19" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>79</v>
@@ -4061,7 +4061,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -4084,16 +4084,16 @@
         <v>90</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="K20" t="s" s="2">
         <v>229</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="L20" t="s" s="2">
         <v>230</v>
       </c>
-      <c r="L20" t="s" s="2">
+      <c r="M20" t="s" s="2">
         <v>231</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>232</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -4143,7 +4143,7 @@
         <v>79</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>77</v>
@@ -4164,13 +4164,13 @@
         <v>79</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>79</v>
@@ -4178,11 +4178,11 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
@@ -4201,19 +4201,19 @@
         <v>90</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="K21" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="K21" t="s" s="2">
+      <c r="L21" t="s" s="2">
         <v>237</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>238</v>
       </c>
-      <c r="M21" t="s" s="2">
+      <c r="N21" t="s" s="2">
         <v>239</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>240</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>79</v>
@@ -4262,7 +4262,7 @@
         <v>79</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>77</v>
@@ -4277,19 +4277,19 @@
         <v>101</v>
       </c>
       <c r="AJ21" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="AK21" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AL21" t="s" s="2">
         <v>241</v>
       </c>
-      <c r="AK21" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AL21" t="s" s="2">
+      <c r="AM21" t="s" s="2">
         <v>242</v>
       </c>
-      <c r="AM21" t="s" s="2">
+      <c r="AN21" t="s" s="2">
         <v>243</v>
-      </c>
-      <c r="AN21" t="s" s="2">
-        <v>244</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>79</v>
@@ -4297,11 +4297,11 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
@@ -4320,19 +4320,19 @@
         <v>90</v>
       </c>
       <c r="J22" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="K22" t="s" s="2">
         <v>247</v>
       </c>
-      <c r="K22" t="s" s="2">
+      <c r="L22" t="s" s="2">
         <v>248</v>
       </c>
-      <c r="L22" t="s" s="2">
+      <c r="M22" t="s" s="2">
         <v>249</v>
       </c>
-      <c r="M22" t="s" s="2">
+      <c r="N22" t="s" s="2">
         <v>250</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>251</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>79</v>
@@ -4381,7 +4381,7 @@
         <v>79</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>77</v>
@@ -4390,25 +4390,25 @@
         <v>89</v>
       </c>
       <c r="AH22" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="AI22" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="AI22" t="s" s="2">
+      <c r="AJ22" t="s" s="2">
         <v>253</v>
       </c>
-      <c r="AJ22" t="s" s="2">
+      <c r="AK22" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AL22" t="s" s="2">
         <v>254</v>
       </c>
-      <c r="AK22" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AL22" t="s" s="2">
+      <c r="AM22" t="s" s="2">
         <v>255</v>
       </c>
-      <c r="AM22" t="s" s="2">
+      <c r="AN22" t="s" s="2">
         <v>256</v>
-      </c>
-      <c r="AN22" t="s" s="2">
-        <v>257</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>79</v>
@@ -4416,7 +4416,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4439,16 +4439,16 @@
         <v>90</v>
       </c>
       <c r="J23" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="K23" t="s" s="2">
         <v>259</v>
       </c>
-      <c r="K23" t="s" s="2">
+      <c r="L23" t="s" s="2">
         <v>260</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>261</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>262</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
@@ -4498,7 +4498,7 @@
         <v>79</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>77</v>
@@ -4519,13 +4519,13 @@
         <v>79</v>
       </c>
       <c r="AL23" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="AM23" t="s" s="2">
         <v>263</v>
       </c>
-      <c r="AM23" t="s" s="2">
+      <c r="AN23" t="s" s="2">
         <v>264</v>
-      </c>
-      <c r="AN23" t="s" s="2">
-        <v>265</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>79</v>
@@ -4533,7 +4533,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4556,19 +4556,19 @@
         <v>90</v>
       </c>
       <c r="J24" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="K24" t="s" s="2">
         <v>267</v>
       </c>
-      <c r="K24" t="s" s="2">
+      <c r="L24" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="L24" t="s" s="2">
+      <c r="M24" t="s" s="2">
         <v>269</v>
       </c>
-      <c r="M24" t="s" s="2">
+      <c r="N24" t="s" s="2">
         <v>270</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>271</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>79</v>
@@ -4617,7 +4617,7 @@
         <v>79</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>77</v>
@@ -4632,19 +4632,19 @@
         <v>101</v>
       </c>
       <c r="AJ24" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="AK24" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AL24" t="s" s="2">
         <v>272</v>
       </c>
-      <c r="AK24" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AL24" t="s" s="2">
+      <c r="AM24" t="s" s="2">
         <v>273</v>
       </c>
-      <c r="AM24" t="s" s="2">
+      <c r="AN24" t="s" s="2">
         <v>274</v>
-      </c>
-      <c r="AN24" t="s" s="2">
-        <v>275</v>
       </c>
       <c r="AO24" t="s" s="2">
         <v>79</v>
@@ -4652,7 +4652,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4675,19 +4675,19 @@
         <v>90</v>
       </c>
       <c r="J25" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="K25" t="s" s="2">
         <v>277</v>
       </c>
-      <c r="K25" t="s" s="2">
+      <c r="L25" t="s" s="2">
         <v>278</v>
       </c>
-      <c r="L25" t="s" s="2">
+      <c r="M25" t="s" s="2">
         <v>279</v>
       </c>
-      <c r="M25" t="s" s="2">
+      <c r="N25" t="s" s="2">
         <v>280</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>281</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>79</v>
@@ -4736,7 +4736,7 @@
         <v>79</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>77</v>
@@ -4745,7 +4745,7 @@
         <v>89</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>101</v>
@@ -4754,24 +4754,24 @@
         <v>79</v>
       </c>
       <c r="AK25" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="AL25" t="s" s="2">
         <v>283</v>
       </c>
-      <c r="AL25" t="s" s="2">
+      <c r="AM25" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="AM25" t="s" s="2">
+      <c r="AN25" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AO25" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="AN25" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AO25" t="s" s="2">
-        <v>286</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4797,16 +4797,16 @@
         <v>187</v>
       </c>
       <c r="K26" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="L26" t="s" s="2">
         <v>288</v>
       </c>
-      <c r="L26" t="s" s="2">
+      <c r="M26" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="M26" t="s" s="2">
+      <c r="N26" t="s" s="2">
         <v>290</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>291</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>79</v>
@@ -4831,7 +4831,7 @@
         <v>79</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>210</v>
+        <v>291</v>
       </c>
       <c r="X26" t="s" s="2">
         <v>292</v>
@@ -4855,7 +4855,7 @@
         <v>79</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>77</v>
@@ -4950,7 +4950,7 @@
         <v>79</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>210</v>
+        <v>291</v>
       </c>
       <c r="X27" t="s" s="2">
         <v>302</v>
@@ -7577,13 +7577,13 @@
         <v>442</v>
       </c>
       <c r="AL49" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="AM49" t="s" s="2">
         <v>214</v>
       </c>
-      <c r="AM49" t="s" s="2">
+      <c r="AN49" t="s" s="2">
         <v>215</v>
-      </c>
-      <c r="AN49" t="s" s="2">
-        <v>216</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>79</v>
@@ -7614,19 +7614,19 @@
         <v>90</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K50" t="s" s="2">
         <v>444</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M50" t="s" s="2">
         <v>445</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>79</v>
@@ -7696,16 +7696,16 @@
         <v>446</v>
       </c>
       <c r="AL50" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="AM50" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="AM50" t="s" s="2">
+      <c r="AN50" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AO50" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="AN50" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AO50" t="s" s="2">
-        <v>286</v>
       </c>
     </row>
     <row r="51" hidden="true">
@@ -7745,7 +7745,7 @@
         <v>450</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>79</v>
@@ -7770,7 +7770,7 @@
         <v>79</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>210</v>
+        <v>291</v>
       </c>
       <c r="X51" t="s" s="2">
         <v>292</v>
@@ -7889,7 +7889,7 @@
         <v>79</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>210</v>
+        <v>291</v>
       </c>
       <c r="X52" t="s" s="2">
         <v>302</v>

</xml_diff>